<commit_message>
atualização do slides 10
</commit_message>
<xml_diff>
--- a/Requisitos/relatorio de avaliação de teste.xlsx
+++ b/Requisitos/relatorio de avaliação de teste.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josimar\Documents\GitHub\SIB\Requisitos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="19440" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Plan2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -78,9 +73,6 @@
     <t>TESTADOR</t>
   </si>
   <si>
-    <t>CONFIG MUD</t>
-  </si>
-  <si>
     <t>LUIS</t>
   </si>
   <si>
@@ -100,6 +92,9 @@
   </si>
   <si>
     <t>12 Horas</t>
+  </si>
+  <si>
+    <t>G.CONFIG MUD</t>
   </si>
 </sst>
 </file>
@@ -271,6 +266,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -279,27 +295,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -361,7 +356,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -396,7 +391,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -608,7 +603,7 @@
   <dimension ref="D2:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +618,7 @@
   <sheetData>
     <row r="2" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="13" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="11"/>
@@ -638,10 +633,10 @@
       <c r="N3" s="12"/>
     </row>
     <row r="4" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="17"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="19"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="16"/>
       <c r="H4" s="1" t="s">
         <v>10</v>
       </c>
@@ -655,7 +650,7 @@
         <v>18</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="2"/>
@@ -669,27 +664,27 @@
         <v>9</v>
       </c>
       <c r="I5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="K5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="L5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
       <c r="H6" s="1" t="s">
         <v>11</v>
       </c>
@@ -697,10 +692,10 @@
         <v>12</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L6" s="8"/>
       <c r="M6" s="1"/>
@@ -798,24 +793,24 @@
       <c r="F11" s="11"/>
       <c r="G11" s="12"/>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="2"/>
     </row>
     <row r="12" spans="4:14" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="22"/>
       <c r="H12" s="1" t="s">
         <v>15</v>
       </c>
@@ -833,12 +828,12 @@
       <c r="N12" s="2"/>
     </row>
     <row r="13" spans="4:14" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="22"/>
       <c r="H13" s="1" t="s">
         <v>14</v>
       </c>
@@ -846,7 +841,7 @@
         <v>14</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>14</v>
@@ -897,17 +892,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D12:G12"/>
     <mergeCell ref="D8:G8"/>
     <mergeCell ref="D3:N3"/>
     <mergeCell ref="D4:G4"/>
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="D6:G6"/>
     <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D12:G12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>